<commit_message>
product interface document update (20190325)
</commit_message>
<xml_diff>
--- a/虚拟机环境.xlsx
+++ b/虚拟机环境.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="40.73.1.192" sheetId="1" r:id="rId1"/>
-    <sheet name="40.73.23.194" sheetId="3" r:id="rId2"/>
-    <sheet name="40.73.0.185" sheetId="2" r:id="rId3"/>
+    <sheet name="40.73.23.194" sheetId="2" r:id="rId2"/>
+    <sheet name="139.217.228.205" sheetId="4" r:id="rId3"/>
+    <sheet name="Nexus" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,12 +22,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
   <si>
     <t>密码</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>qeWf25?Bo</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>应用</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -52,6 +57,10 @@
   </si>
   <si>
     <t>root</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>m]eaxXbeds73Nuki</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -180,15 +189,34 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>qeWf25?Bo</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>m]eaxXbeds73Nuki</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>permanent disk</t>
+    <t>http://139.217.235.112:8081/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>liangbo@nissanchina.cn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mfyJD27o</t>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mysql</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Permanent  disk</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -196,7 +224,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">/project  </t>
+    <t>A8oG8CO8VOdmggpm</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -204,7 +232,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +261,14 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -282,7 +318,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -290,6 +326,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -302,6 +339,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,12 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -325,13 +360,82 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="标题 2" xfId="1" builtinId="17"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8"/>
     <cellStyle name="注释" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -351,7 +455,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="DCEACE"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -606,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -626,171 +730,163 @@
       <c r="A1" s="3"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1">
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>8080</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1">
         <v>443</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
+      <c r="A7" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
         <v>3306</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>20</v>
+      <c r="A8" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1">
         <v>6379</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
+      <c r="A9" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1">
         <v>27017</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A3:A4"/>
@@ -804,142 +900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.08203125" customWidth="1"/>
-    <col min="2" max="2" width="16.08203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="35.25" customWidth="1"/>
-    <col min="6" max="6" width="34.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="1">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="9">
-        <v>8080</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="9">
-        <v>443</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-  </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -956,119 +920,127 @@
       <c r="A1" s="3"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1">
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1">
         <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2">
         <v>8080</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>38</v>
+      <c r="E5" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2">
         <v>443</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D7" s="1">
         <v>3306</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:6" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:A4"/>
@@ -1078,4 +1050,195 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.4140625" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="43.4140625" customWidth="1"/>
+    <col min="4" max="4" width="17.9140625" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="30.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8080</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="4">
+        <v>443</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3306</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update project document files
</commit_message>
<xml_diff>
--- a/虚拟机环境.xlsx
+++ b/虚拟机环境.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="0" windowHeight="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="40.73.1.192" sheetId="1" r:id="rId1"/>
     <sheet name="40.73.23.194" sheetId="2" r:id="rId2"/>
     <sheet name="139.217.228.205" sheetId="4" r:id="rId3"/>
     <sheet name="Nexus" sheetId="5" r:id="rId4"/>
+    <sheet name="Jenkins" sheetId="6" r:id="rId5"/>
+    <sheet name="aliyun" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>密码</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -165,10 +167,6 @@
   </si>
   <si>
     <t>域名: evtest.nissan.china.cn</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>obuR1MVKhGP5</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -189,42 +187,85 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>admin</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mysql</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Permanent  disk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A8oG8CO8VOdmggpm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>liangbo@nissanchina.cn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mfyJD27o</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>http://139.217.235.112:8081/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>liangbo@nissanchina.cn</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mfyJD27o</t>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>password</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>url</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mysql</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Permanent  disk</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>A8oG8CO8VOdmggpm</t>
+    <t>obuR1MVKhGP5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>jenkins:  https://jenkins.nissan.com.cn/
+account: devops
+password: 8CnFAb@2xgL9O2&amp;*</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">account: </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>devops</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">password: </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FX9X8el*KLCo!JcB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://signin.aliyun.com/1615541751802351.onaliyun.com/login.htm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>account</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>devops@1615541751802351.onaliyun.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4ZH7Pkp$9Zaa#Pp5</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -328,7 +369,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -359,6 +400,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="标题 2" xfId="1" builtinId="17"/>
@@ -368,74 +415,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -713,7 +692,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -902,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -948,7 +927,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1">
         <v>22</v>
@@ -966,7 +945,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1">
         <v>22</v>
@@ -986,13 +965,13 @@
         <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2">
         <v>8080</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
@@ -1002,13 +981,13 @@
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2">
         <v>443</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>17</v>
@@ -1022,7 +1001,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1">
         <v>3306</v>
@@ -1034,10 +1013,10 @@
     </row>
     <row r="8" spans="1:6" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1056,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1102,7 +1081,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1">
         <v>22</v>
@@ -1130,13 +1109,13 @@
         <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="4">
         <v>8080</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
@@ -1146,13 +1125,13 @@
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="4">
         <v>443</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>17</v>
@@ -1160,13 +1139,13 @@
     </row>
     <row r="7" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1">
         <v>3306</v>
@@ -1178,10 +1157,10 @@
     </row>
     <row r="8" spans="1:6" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1198,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="H15" sqref="H15:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1211,26 +1190,118 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="12"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="62.4140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="42" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="57.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>